<commit_message>
fixing 1000 to 850, due to duplicates
</commit_message>
<xml_diff>
--- a/Results/AreasofDisturbance_ceoV4version_SAVE.xlsx
+++ b/Results/AreasofDisturbance_ceoV4version_SAVE.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e0c35774a9514c4a/Documents/Philippines/PhilippinesQAQCanalysis/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AC1D2DB8-58FC-415D-9C09-9A26936B2E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{AC1D2DB8-58FC-415D-9C09-9A26936B2E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8904F04C-60D4-4F43-B117-CBA36BD49567}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460"/>
+    <workbookView xWindow="7305" yWindow="1215" windowWidth="18815" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AreasofDisturbance_ceoV4version" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Total, ha</t>
-  </si>
-  <si>
-    <t>SE, ha</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Deforestation</t>
   </si>
@@ -48,14 +42,23 @@
   <si>
     <t>stable non-forest agroforestry</t>
   </si>
+  <si>
+    <t>Strata</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -543,7 +546,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -900,11 +903,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -915,16 +918,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>860706</v>
@@ -935,7 +941,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>729675</v>
@@ -946,7 +952,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>198067</v>
@@ -957,7 +963,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>674458</v>
@@ -968,7 +974,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>7961169</v>
@@ -979,7 +985,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>14382249</v>
@@ -990,7 +996,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>4930003</v>

</xml_diff>